<commit_message>
cn-#5 add converter step
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38107619-39CC-474D-ADBA-26679F359453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782C6624-5555-4443-AA0B-F3BB0CB9F39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTest" sheetId="1" r:id="rId1"/>
@@ -386,14 +386,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,8 +442,8 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <f>C2+C3</f>
-        <v>120</v>
+        <f>C2+C3+1000</f>
+        <v>1120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cn-#5 first sample test
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782C6624-5555-4443-AA0B-F3BB0CB9F39C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7425A8-716F-48DB-9288-B2ED3DF15E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,8 +442,8 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <f>C2+C3+1000</f>
-        <v>1120</v>
+        <f>C2+C3</f>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cn-#5 format diff result display
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7425A8-716F-48DB-9288-B2ED3DF15E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F362DFB5-6B96-4952-B2E2-190C16DA205B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,14 +434,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <f>C2+C3</f>
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
cn-#13 test Each Sheet is a scenario
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/SampleTest.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E820FEC-AE9C-4448-8B51-195BD6C9B29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ACDE29-51F4-4808-9C10-6720F2A582E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SampleTest" sheetId="1" r:id="rId1"/>
+    <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
+    <sheet name="MinusTwoNumbers" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Scenario</t>
   </si>
@@ -66,6 +67,12 @@
   </si>
   <si>
     <t>the result should be</t>
+  </si>
+  <si>
+    <t>Minus  two numbers</t>
+  </si>
+  <si>
+    <t>I subtract the second number from the first number</t>
   </si>
 </sst>
 </file>
@@ -385,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,4 +456,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A846831B-4BF8-4D53-81F0-A1BB81F576E3}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <f>C2-C3</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>